<commit_message>
admin pages, get method
</commit_message>
<xml_diff>
--- a/Planejamento-IFBOOKS-4ano-informatica-joao_eduardo_nathan.xlsx
+++ b/Planejamento-IFBOOKS-4ano-informatica-joao_eduardo_nathan.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Joao_2\OneDrive\Documentos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\TCC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4A8B644-B7C8-42F7-9A33-B1F2D06E809F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF28E068-824C-4786-9CBD-6C7D012B296A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="11040" xr2:uid="{9EC0FD2E-D50E-47A5-B7F4-2A601CFD3F30}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
   <si>
     <t>Atividade Planejada</t>
   </si>
@@ -82,6 +82,9 @@
   </si>
   <si>
     <t>João Pedro Romão, Nathan Guido, Eduardo Julião</t>
+  </si>
+  <si>
+    <t>https://youtu.be/JILqNlTV-8k</t>
   </si>
 </sst>
 </file>
@@ -150,7 +153,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -182,7 +185,6 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hiperlink" xfId="1" builtinId="8"/>
@@ -501,7 +503,7 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -582,7 +584,9 @@
       <c r="A10" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="11"/>
+      <c r="B10" s="7" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="11" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
@@ -595,8 +599,9 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B11" r:id="rId1" xr:uid="{78318969-89F8-4C41-ADE8-640B4D351C0E}"/>
+    <hyperlink ref="B10" r:id="rId2" xr:uid="{9DFAA9CE-B6C0-428C-B85E-4BE5EB1CE061}"/>
   </hyperlinks>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>